<commit_message>
errata corrige pp e scrum
</commit_message>
<xml_diff>
--- a/02_DOCUMENTATION/SCRUM MEDITREX.xlsx
+++ b/02_DOCUMENTATION/SCRUM MEDITREX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\GitHub\MediTrex\02_DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50172AFC-76F9-40D5-B572-86C74AF84368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF52248-8101-405D-8686-47DBC57AB4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23100" yWindow="2835" windowWidth="27600" windowHeight="16980" tabRatio="237" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="237" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -1695,6 +1695,30 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1727,30 +1751,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2018,7 +2018,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt Chart &amp; Burndown'!$M$24:$BE$24</c15:sqref>
+                    <c15:sqref>'Gantt Chart &amp; Burndown'!$M$24:$AP$24</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
@@ -2124,7 +2124,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt Chart &amp; Burndown'!$M$25:$BE$25</c15:sqref>
+                    <c15:sqref>'Gantt Chart &amp; Burndown'!$M$25:$AP$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
@@ -2136,91 +2136,91 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.36363636363637</c:v>
+                  <c:v>154.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>152.72727272727275</c:v>
+                  <c:v>149.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149.09090909090912</c:v>
+                  <c:v>143.99999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>145.4545454545455</c:v>
+                  <c:v>138.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>141.81818181818187</c:v>
+                  <c:v>133.33333333333329</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>138.18181818181824</c:v>
+                  <c:v>127.99999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>134.54545454545462</c:v>
+                  <c:v>122.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130.90909090909099</c:v>
+                  <c:v>117.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>127.27272727272735</c:v>
+                  <c:v>111.99999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>123.63636363636371</c:v>
+                  <c:v>106.66666666666664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>120.00000000000007</c:v>
+                  <c:v>101.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>116.36363636363643</c:v>
+                  <c:v>95.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>112.72727272727279</c:v>
+                  <c:v>90.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>109.09090909090915</c:v>
+                  <c:v>85.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>105.45454545454551</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>101.81818181818187</c:v>
+                  <c:v>74.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>98.18181818181823</c:v>
+                  <c:v>69.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>94.545454545454589</c:v>
+                  <c:v>64.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>90.909090909090949</c:v>
+                  <c:v>58.666666666666679</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>87.272727272727309</c:v>
+                  <c:v>53.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>83.636363636363669</c:v>
+                  <c:v>48.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>80.000000000000028</c:v>
+                  <c:v>42.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>76.363636363636388</c:v>
+                  <c:v>37.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>72.727272727272748</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>69.090909090909108</c:v>
+                  <c:v>26.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>65.454545454545467</c:v>
+                  <c:v>21.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>61.818181818181834</c:v>
+                  <c:v>16.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>58.181818181818201</c:v>
+                  <c:v>10.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>54.545454545454568</c:v>
+                  <c:v>5.3333333333333384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2407,91 +2407,91 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>158</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>155</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>150</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>142</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>134</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>127</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>115</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>95</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>90</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>85</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>79</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>73</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>66</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>46</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>35</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2647,94 +2647,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>158</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>155</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>142</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>134</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>127</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>120</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>115</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>105</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>95</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>90</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>85</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>79</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>73</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>66</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>46</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3406,8 +3406,8 @@
   </sheetPr>
   <dimension ref="B1:BG39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO16" sqref="AO16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3511,7 +3511,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="123" t="s">
+      <c r="K3" s="133" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="7" t="s">
@@ -3573,7 +3573,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="124"/>
+      <c r="K4" s="134"/>
       <c r="L4" s="11" t="s">
         <v>4</v>
       </c>
@@ -3633,7 +3633,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="124"/>
+      <c r="K5" s="134"/>
       <c r="L5" s="15" t="s">
         <v>5</v>
       </c>
@@ -3684,75 +3684,75 @@
       <c r="BE5" s="2"/>
     </row>
     <row r="6" spans="2:59" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="127" t="s">
+      <c r="C6" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="129" t="s">
+      <c r="D6" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="131" t="s">
+      <c r="E6" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="132"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="136" t="s">
+      <c r="F6" s="142"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="140" t="s">
+      <c r="J6" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="142" t="s">
+      <c r="K6" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="143" t="s">
+      <c r="L6" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="145" t="s">
+      <c r="M6" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="146"/>
-      <c r="O6" s="146"/>
-      <c r="P6" s="146"/>
-      <c r="Q6" s="146"/>
-      <c r="R6" s="146" t="s">
+      <c r="N6" s="130"/>
+      <c r="O6" s="130"/>
+      <c r="P6" s="130"/>
+      <c r="Q6" s="130"/>
+      <c r="R6" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="S6" s="146"/>
-      <c r="T6" s="146"/>
-      <c r="U6" s="146"/>
-      <c r="V6" s="146"/>
-      <c r="W6" s="147" t="s">
+      <c r="S6" s="130"/>
+      <c r="T6" s="130"/>
+      <c r="U6" s="130"/>
+      <c r="V6" s="130"/>
+      <c r="W6" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="X6" s="147"/>
-      <c r="Y6" s="147"/>
-      <c r="Z6" s="147"/>
-      <c r="AA6" s="147"/>
-      <c r="AB6" s="147" t="s">
+      <c r="X6" s="131"/>
+      <c r="Y6" s="131"/>
+      <c r="Z6" s="131"/>
+      <c r="AA6" s="131"/>
+      <c r="AB6" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="AC6" s="147"/>
-      <c r="AD6" s="147"/>
-      <c r="AE6" s="147"/>
-      <c r="AF6" s="147"/>
-      <c r="AG6" s="122" t="s">
+      <c r="AC6" s="131"/>
+      <c r="AD6" s="131"/>
+      <c r="AE6" s="131"/>
+      <c r="AF6" s="131"/>
+      <c r="AG6" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="AH6" s="122"/>
-      <c r="AI6" s="122"/>
-      <c r="AJ6" s="122"/>
-      <c r="AK6" s="122"/>
-      <c r="AL6" s="122" t="s">
+      <c r="AH6" s="132"/>
+      <c r="AI6" s="132"/>
+      <c r="AJ6" s="132"/>
+      <c r="AK6" s="132"/>
+      <c r="AL6" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="AM6" s="122"/>
-      <c r="AN6" s="122"/>
-      <c r="AO6" s="122"/>
-      <c r="AP6" s="122"/>
+      <c r="AM6" s="132"/>
+      <c r="AN6" s="132"/>
+      <c r="AO6" s="132"/>
+      <c r="AP6" s="132"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
@@ -3770,9 +3770,9 @@
       <c r="BE6" s="2"/>
     </row>
     <row r="7" spans="2:59" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="126"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="130"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="140"/>
       <c r="E7" s="17" t="s">
         <v>21</v>
       </c>
@@ -3782,11 +3782,11 @@
       <c r="G7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="135"/>
-      <c r="I7" s="137"/>
-      <c r="J7" s="141"/>
-      <c r="K7" s="141"/>
-      <c r="L7" s="144"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="128"/>
       <c r="M7" s="87" t="s">
         <v>24</v>
       </c>
@@ -5274,12 +5274,11 @@
         <v>0</v>
       </c>
       <c r="H24" s="86">
-        <f>SUM(K9:K22)</f>
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="I24" s="50">
         <f>E24/H24</f>
-        <v>3.6363636363636362</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="L24" s="100" t="s">
         <v>34</v>
@@ -5402,119 +5401,119 @@
       </c>
       <c r="N25" s="54">
         <f>M25-I24</f>
-        <v>156.36363636363637</v>
+        <v>154.66666666666666</v>
       </c>
       <c r="O25" s="54">
         <f>N25-I24</f>
-        <v>152.72727272727275</v>
+        <v>149.33333333333331</v>
       </c>
       <c r="P25" s="54">
         <f>O25-I24</f>
-        <v>149.09090909090912</v>
+        <v>143.99999999999997</v>
       </c>
       <c r="Q25" s="54">
         <f>P25-I24</f>
-        <v>145.4545454545455</v>
+        <v>138.66666666666663</v>
       </c>
       <c r="R25" s="54">
         <f>Q25-I24</f>
-        <v>141.81818181818187</v>
+        <v>133.33333333333329</v>
       </c>
       <c r="S25" s="54">
         <f>R25-I24</f>
-        <v>138.18181818181824</v>
+        <v>127.99999999999996</v>
       </c>
       <c r="T25" s="54">
         <f>S25-I24</f>
-        <v>134.54545454545462</v>
+        <v>122.66666666666663</v>
       </c>
       <c r="U25" s="54">
         <f>T25-I24</f>
-        <v>130.90909090909099</v>
+        <v>117.3333333333333</v>
       </c>
       <c r="V25" s="54">
         <f>U25-I24</f>
-        <v>127.27272727272735</v>
+        <v>111.99999999999997</v>
       </c>
       <c r="W25" s="54">
         <f>V25-I24</f>
-        <v>123.63636363636371</v>
+        <v>106.66666666666664</v>
       </c>
       <c r="X25" s="54">
         <f>W25-I24</f>
-        <v>120.00000000000007</v>
+        <v>101.33333333333331</v>
       </c>
       <c r="Y25" s="54">
         <f>X25-I24</f>
-        <v>116.36363636363643</v>
+        <v>95.999999999999986</v>
       </c>
       <c r="Z25" s="54">
         <f>Y25-I24</f>
-        <v>112.72727272727279</v>
+        <v>90.666666666666657</v>
       </c>
       <c r="AA25" s="54">
         <f>Z25-I24</f>
-        <v>109.09090909090915</v>
+        <v>85.333333333333329</v>
       </c>
       <c r="AB25" s="54">
         <f>AA25-I24</f>
-        <v>105.45454545454551</v>
+        <v>80</v>
       </c>
       <c r="AC25" s="54">
         <f>AB25-I24</f>
-        <v>101.81818181818187</v>
+        <v>74.666666666666671</v>
       </c>
       <c r="AD25" s="54">
         <f>AC25-I24</f>
-        <v>98.18181818181823</v>
+        <v>69.333333333333343</v>
       </c>
       <c r="AE25" s="54">
         <f>AD25-I24</f>
-        <v>94.545454545454589</v>
+        <v>64.000000000000014</v>
       </c>
       <c r="AF25" s="54">
         <f>AE25-I24</f>
-        <v>90.909090909090949</v>
+        <v>58.666666666666679</v>
       </c>
       <c r="AG25" s="54">
         <f>AF25-I24</f>
-        <v>87.272727272727309</v>
+        <v>53.333333333333343</v>
       </c>
       <c r="AH25" s="54">
         <f>AG25-I24</f>
-        <v>83.636363636363669</v>
+        <v>48.000000000000007</v>
       </c>
       <c r="AI25" s="54">
         <f>AH25-I24</f>
-        <v>80.000000000000028</v>
+        <v>42.666666666666671</v>
       </c>
       <c r="AJ25" s="54">
         <f>AI25-I24</f>
-        <v>76.363636363636388</v>
+        <v>37.333333333333336</v>
       </c>
       <c r="AK25" s="54">
         <f>AJ25-I24</f>
-        <v>72.727272727272748</v>
+        <v>32</v>
       </c>
       <c r="AL25" s="54">
         <f>AK25-I24</f>
-        <v>69.090909090909108</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="AM25" s="54">
         <f>AL25-I24</f>
-        <v>65.454545454545467</v>
+        <v>21.333333333333336</v>
       </c>
       <c r="AN25" s="54">
         <f>AM25-I24</f>
-        <v>61.818181818181834</v>
+        <v>16.000000000000004</v>
       </c>
       <c r="AO25" s="54">
         <f>AN25-I24</f>
-        <v>58.181818181818201</v>
+        <v>10.666666666666671</v>
       </c>
       <c r="AP25" s="54">
         <f>AO25-I24</f>
-        <v>54.545454545454568</v>
+        <v>5.3333333333333384</v>
       </c>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
@@ -5544,119 +5543,119 @@
       </c>
       <c r="N26" s="53">
         <f t="shared" ref="N26:AP26" si="7">M28</f>
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O26" s="53">
         <f t="shared" si="7"/>
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="P26" s="53">
         <f t="shared" si="7"/>
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Q26" s="53">
         <f t="shared" si="7"/>
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="R26" s="53">
         <f t="shared" si="7"/>
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="S26" s="53">
         <f t="shared" si="7"/>
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="T26" s="53">
         <f t="shared" si="7"/>
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="U26" s="53">
         <f t="shared" si="7"/>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V26" s="53">
         <f t="shared" si="7"/>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="W26" s="53">
         <f t="shared" si="7"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="X26" s="53">
         <f t="shared" si="7"/>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Y26" s="53">
         <f t="shared" si="7"/>
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Z26" s="53">
         <f t="shared" si="7"/>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AA26" s="53">
         <f t="shared" si="7"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB26" s="53">
         <f t="shared" si="7"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AC26" s="53">
         <f t="shared" si="7"/>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AD26" s="53">
         <f t="shared" si="7"/>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AE26" s="53">
         <f t="shared" si="7"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF26" s="53">
         <f t="shared" si="7"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AG26" s="53">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AH26" s="53">
         <f t="shared" si="7"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AI26" s="53">
         <f t="shared" si="7"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AJ26" s="53">
         <f t="shared" si="7"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AK26" s="53">
         <f t="shared" si="7"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AL26" s="53">
         <f t="shared" si="7"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AM26" s="53">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AN26" s="53">
         <f t="shared" si="7"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AO26" s="53">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AP26" s="53">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
@@ -5682,43 +5681,35 @@
         <v>36</v>
       </c>
       <c r="M27" s="102">
-        <f>SUM(M9:M22)</f>
         <v>1</v>
       </c>
       <c r="N27" s="102">
-        <f t="shared" ref="N27:AP27" si="8">SUM(N9:N22)</f>
         <v>1</v>
       </c>
       <c r="O27" s="102">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P27" s="102">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q27" s="102">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="R27" s="102">
-        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="S27" s="102">
-        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="T27" s="102">
-        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="U27" s="102">
-        <f t="shared" si="8"/>
+        <f>SUM(U9:U22)</f>
         <v>7</v>
       </c>
       <c r="V27" s="102">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="N27:AP27" si="8">SUM(V9:V22)</f>
         <v>7</v>
       </c>
       <c r="W27" s="102">
@@ -5823,125 +5814,124 @@
       <c r="L28" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="53">
-        <f t="shared" ref="M28:AP28" si="9">M26-M27</f>
+      <c r="M28" s="102">
+        <v>160</v>
+      </c>
+      <c r="N28" s="53">
+        <f t="shared" ref="M28:AP28" si="9">N26-N27</f>
         <v>159</v>
       </c>
-      <c r="N28" s="53">
+      <c r="O28" s="53">
         <f t="shared" si="9"/>
         <v>158</v>
       </c>
-      <c r="O28" s="53">
+      <c r="P28" s="53">
         <f t="shared" si="9"/>
         <v>157</v>
       </c>
-      <c r="P28" s="53">
+      <c r="Q28" s="53">
         <f t="shared" si="9"/>
         <v>156</v>
       </c>
-      <c r="Q28" s="53">
-        <f t="shared" si="9"/>
-        <v>155</v>
-      </c>
       <c r="R28" s="53">
         <f t="shared" si="9"/>
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="S28" s="53">
         <f t="shared" si="9"/>
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="T28" s="53">
         <f t="shared" si="9"/>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="U28" s="53">
         <f t="shared" si="9"/>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="V28" s="53">
         <f t="shared" si="9"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="W28" s="53">
         <f t="shared" si="9"/>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="X28" s="53">
         <f t="shared" si="9"/>
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Y28" s="53">
         <f t="shared" si="9"/>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Z28" s="53">
         <f t="shared" si="9"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AA28" s="53">
         <f t="shared" si="9"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AB28" s="53">
         <f t="shared" si="9"/>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AC28" s="53">
         <f t="shared" si="9"/>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD28" s="53">
         <f t="shared" si="9"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AE28" s="53">
         <f t="shared" si="9"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AF28" s="53">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG28" s="53">
         <f t="shared" si="9"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH28" s="53">
         <f t="shared" si="9"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI28" s="53">
         <f t="shared" si="9"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AJ28" s="53">
         <f t="shared" si="9"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AK28" s="53">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AL28" s="53">
         <f t="shared" si="9"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AM28" s="53">
         <f t="shared" si="9"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AN28" s="53">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AO28" s="53">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AP28" s="53">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ28" s="2"/>
       <c r="AR28" s="2"/>
@@ -5982,62 +5972,62 @@
     <row r="30" spans="2:59" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:59" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="138"/>
-      <c r="C32" s="139"/>
-      <c r="D32" s="139"/>
-      <c r="E32" s="139"/>
-      <c r="F32" s="139"/>
-      <c r="G32" s="139"/>
-      <c r="H32" s="139"/>
-      <c r="I32" s="139"/>
-      <c r="J32" s="139"/>
-      <c r="K32" s="139"/>
-      <c r="L32" s="139"/>
-      <c r="M32" s="139"/>
-      <c r="N32" s="139"/>
-      <c r="O32" s="139"/>
-      <c r="P32" s="139"/>
-      <c r="Q32" s="139"/>
-      <c r="R32" s="139"/>
-      <c r="S32" s="139"/>
-      <c r="T32" s="139"/>
-      <c r="U32" s="139"/>
-      <c r="V32" s="139"/>
-      <c r="W32" s="139"/>
-      <c r="X32" s="139"/>
-      <c r="Y32" s="139"/>
-      <c r="Z32" s="139"/>
-      <c r="AA32" s="139"/>
-      <c r="AB32" s="139"/>
-      <c r="AC32" s="139"/>
-      <c r="AD32" s="139"/>
-      <c r="AE32" s="139"/>
-      <c r="AF32" s="139"/>
-      <c r="AG32" s="139"/>
-      <c r="AH32" s="139"/>
-      <c r="AI32" s="139"/>
-      <c r="AJ32" s="139"/>
-      <c r="AK32" s="139"/>
-      <c r="AL32" s="139"/>
-      <c r="AM32" s="139"/>
-      <c r="AN32" s="139"/>
-      <c r="AO32" s="139"/>
-      <c r="AP32" s="139"/>
-      <c r="AQ32" s="139"/>
-      <c r="AR32" s="139"/>
-      <c r="AS32" s="139"/>
-      <c r="AT32" s="139"/>
-      <c r="AU32" s="139"/>
-      <c r="AV32" s="139"/>
-      <c r="AW32" s="139"/>
-      <c r="AX32" s="139"/>
-      <c r="AY32" s="139"/>
-      <c r="AZ32" s="139"/>
-      <c r="BA32" s="139"/>
-      <c r="BB32" s="139"/>
-      <c r="BC32" s="139"/>
-      <c r="BD32" s="139"/>
-      <c r="BE32" s="139"/>
+      <c r="B32" s="122"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="123"/>
+      <c r="K32" s="123"/>
+      <c r="L32" s="123"/>
+      <c r="M32" s="123"/>
+      <c r="N32" s="123"/>
+      <c r="O32" s="123"/>
+      <c r="P32" s="123"/>
+      <c r="Q32" s="123"/>
+      <c r="R32" s="123"/>
+      <c r="S32" s="123"/>
+      <c r="T32" s="123"/>
+      <c r="U32" s="123"/>
+      <c r="V32" s="123"/>
+      <c r="W32" s="123"/>
+      <c r="X32" s="123"/>
+      <c r="Y32" s="123"/>
+      <c r="Z32" s="123"/>
+      <c r="AA32" s="123"/>
+      <c r="AB32" s="123"/>
+      <c r="AC32" s="123"/>
+      <c r="AD32" s="123"/>
+      <c r="AE32" s="123"/>
+      <c r="AF32" s="123"/>
+      <c r="AG32" s="123"/>
+      <c r="AH32" s="123"/>
+      <c r="AI32" s="123"/>
+      <c r="AJ32" s="123"/>
+      <c r="AK32" s="123"/>
+      <c r="AL32" s="123"/>
+      <c r="AM32" s="123"/>
+      <c r="AN32" s="123"/>
+      <c r="AO32" s="123"/>
+      <c r="AP32" s="123"/>
+      <c r="AQ32" s="123"/>
+      <c r="AR32" s="123"/>
+      <c r="AS32" s="123"/>
+      <c r="AT32" s="123"/>
+      <c r="AU32" s="123"/>
+      <c r="AV32" s="123"/>
+      <c r="AW32" s="123"/>
+      <c r="AX32" s="123"/>
+      <c r="AY32" s="123"/>
+      <c r="AZ32" s="123"/>
+      <c r="BA32" s="123"/>
+      <c r="BB32" s="123"/>
+      <c r="BC32" s="123"/>
+      <c r="BD32" s="123"/>
+      <c r="BE32" s="123"/>
     </row>
     <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6045,6 +6035,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="B32:BE32"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
@@ -6055,16 +6052,12 @@
     <mergeCell ref="AB6:AF6"/>
     <mergeCell ref="AG6:AK6"/>
     <mergeCell ref="AL6:AP6"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="U27 V27:AP27" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -6077,7 +6070,7 @@
   </sheetPr>
   <dimension ref="A1:H979"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>